<commit_message>
adding if else statement to deal with georeferencing discrepancies between verbatim and assigned. Also added page number to occurrenceID
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
+++ b/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD4FC98-5288-5B4D-8873-F7106E0DCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E92CF0-EC30-D342-9027-A894AD92A5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15860" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="236">
   <si>
     <t>genus</t>
   </si>
@@ -477,9 +477,6 @@
     <t>not sure if "n" or "m" in Claramo/ Clarano</t>
   </si>
   <si>
-    <t xml:space="preserve">cannot understand Clar amo + inshade </t>
-  </si>
-  <si>
     <t>Osmorhiza berteroi was previously chilensis. Recent iNat observations on Mt. Sutil</t>
   </si>
   <si>
@@ -531,9 +528,6 @@
     <t>vSciName</t>
   </si>
   <si>
-    <t>Clar amo + inshade</t>
-  </si>
-  <si>
     <t>Osmorhiza berteroi</t>
   </si>
   <si>
@@ -876,9 +870,6 @@
     <t>HJ-27-2</t>
   </si>
   <si>
-    <t>HJ-27-3</t>
-  </si>
-  <si>
     <t>HJ-27-4</t>
   </si>
   <si>
@@ -1060,6 +1051,9 @@
   </si>
   <si>
     <t>HJ-27-64</t>
+  </si>
+  <si>
+    <t>in shade</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AB65"/>
+  <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>38</v>
@@ -1618,7 +1612,7 @@
     </row>
     <row r="2" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1662,6 +1656,7 @@
       <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="U2"/>
       <c r="W2" s="4" t="s">
         <v>34</v>
       </c>
@@ -1674,7 +1669,7 @@
     </row>
     <row r="3" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1718,6 +1713,10 @@
       <c r="O3" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="U3"/>
+      <c r="W3" s="4" t="s">
+        <v>235</v>
+      </c>
       <c r="X3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1727,17 +1726,26 @@
     </row>
     <row r="4" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1765,28 +1773,25 @@
       <c r="X4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB4" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="5" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>23</v>
@@ -1818,25 +1823,28 @@
       <c r="X5" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="AB5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
@@ -1874,22 +1882,22 @@
     </row>
     <row r="7" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>23</v>
@@ -1921,28 +1929,28 @@
       <c r="X7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB7" t="s">
-        <v>45</v>
+      <c r="AB7" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>23</v>
@@ -1974,28 +1982,26 @@
       <c r="X8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB8" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AB8"/>
     </row>
     <row r="9" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>23</v>
@@ -2027,11 +2033,13 @@
       <c r="X9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2043,7 +2051,7 @@
         <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>64</v>
@@ -2079,27 +2087,27 @@
         <v>31</v>
       </c>
       <c r="AB10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
         <v>67</v>
-      </c>
-      <c r="F11" t="s">
-        <v>66</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -2128,16 +2136,19 @@
       <c r="O11" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="R11" t="s">
+        <v>92</v>
+      </c>
       <c r="X11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2152,7 +2163,7 @@
         <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>23</v>
@@ -2181,34 +2192,38 @@
       <c r="O12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R12" t="s">
-        <v>94</v>
+      <c r="P12"/>
+      <c r="R12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>23</v>
@@ -2237,35 +2252,32 @@
       <c r="O13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P13"/>
-      <c r="R13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="W13" s="4" t="s">
-        <v>98</v>
+      <c r="R13" t="s">
+        <v>92</v>
+      </c>
+      <c r="W13" t="s">
+        <v>95</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB13" t="s">
-        <v>45</v>
-      </c>
+      <c r="AB13"/>
     </row>
     <row r="14" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
         <v>75</v>
@@ -2277,10 +2289,10 @@
         <v>20</v>
       </c>
       <c r="I14" s="4">
-        <v>20040212</v>
+        <v>20040312</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>25</v>
@@ -2298,34 +2310,33 @@
         <v>29</v>
       </c>
       <c r="R14" t="s">
-        <v>94</v>
-      </c>
-      <c r="W14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB14"/>
+      <c r="AB14" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>23</v>
@@ -2355,33 +2366,33 @@
         <v>29</v>
       </c>
       <c r="R15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>23</v>
@@ -2411,33 +2422,33 @@
         <v>29</v>
       </c>
       <c r="R16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>23</v>
@@ -2467,7 +2478,7 @@
         <v>29</v>
       </c>
       <c r="R17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X17" s="4" t="s">
         <v>31</v>
@@ -2478,16 +2489,16 @@
     </row>
     <row r="18" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -2523,33 +2534,33 @@
         <v>29</v>
       </c>
       <c r="R18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>23</v>
@@ -2579,33 +2590,33 @@
         <v>29</v>
       </c>
       <c r="R19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>23</v>
@@ -2635,33 +2646,33 @@
         <v>29</v>
       </c>
       <c r="R20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>23</v>
@@ -2691,33 +2702,33 @@
         <v>29</v>
       </c>
       <c r="R21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>23</v>
@@ -2747,33 +2758,33 @@
         <v>29</v>
       </c>
       <c r="R22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X22" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>23</v>
@@ -2803,33 +2814,33 @@
         <v>29</v>
       </c>
       <c r="R23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X23" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>23</v>
@@ -2859,36 +2870,36 @@
         <v>29</v>
       </c>
       <c r="R24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
         <v>83</v>
       </c>
-      <c r="D25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>20</v>
@@ -2915,36 +2926,34 @@
         <v>29</v>
       </c>
       <c r="R25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="X25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB25" t="s">
-        <v>48</v>
-      </c>
+      <c r="AB25"/>
     </row>
     <row r="26" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
         <v>85</v>
       </c>
-      <c r="F26" t="s">
-        <v>99</v>
-      </c>
       <c r="G26" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>20</v>
@@ -2971,16 +2980,18 @@
         <v>29</v>
       </c>
       <c r="R26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB26"/>
-    </row>
-    <row r="27" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="AB26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2992,7 +3003,7 @@
         <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
         <v>87</v>
@@ -3024,19 +3035,19 @@
       <c r="O27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R27" t="s">
-        <v>96</v>
+      <c r="R27" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="X27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -3048,7 +3059,7 @@
         <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
         <v>89</v>
@@ -3081,36 +3092,36 @@
         <v>29</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="X28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AB28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>20</v>
@@ -3137,33 +3148,30 @@
         <v>29</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
         <v>102</v>
       </c>
-      <c r="D30" t="s">
-        <v>101</v>
-      </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
@@ -3193,30 +3201,33 @@
         <v>29</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="W30" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" t="s">
-        <v>104</v>
+      <c r="C31" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
@@ -3245,34 +3256,28 @@
       <c r="O31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R31" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="W31" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="X31" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
@@ -3307,7 +3312,7 @@
     </row>
     <row r="33" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -3316,16 +3321,16 @@
         <v>106</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>20</v>
@@ -3350,6 +3355,9 @@
       </c>
       <c r="O33" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>31</v>
@@ -3357,25 +3365,25 @@
     </row>
     <row r="34" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>20</v>
@@ -3402,7 +3410,7 @@
         <v>29</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="X34" s="4" t="s">
         <v>31</v>
@@ -3410,16 +3418,16 @@
     </row>
     <row r="35" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>40</v>
@@ -3428,7 +3436,7 @@
         <v>115</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>20</v>
@@ -3455,7 +3463,7 @@
         <v>29</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>31</v>
@@ -3463,25 +3471,25 @@
     </row>
     <row r="36" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="D36" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>117</v>
+      <c r="F36" t="s">
+        <v>118</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>20</v>
@@ -3506,9 +3514,6 @@
       </c>
       <c r="O36" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="R36" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>31</v>
@@ -3516,7 +3521,7 @@
     </row>
     <row r="37" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -3566,7 +3571,7 @@
     </row>
     <row r="38" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -3616,7 +3621,7 @@
     </row>
     <row r="39" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -3625,13 +3630,13 @@
         <v>123</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
         <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>23</v>
@@ -3666,22 +3671,22 @@
     </row>
     <row r="40" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
       <c r="C40" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" t="s">
         <v>125</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
       </c>
       <c r="E40" t="s">
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>23</v>
@@ -3716,22 +3721,22 @@
     </row>
     <row r="41" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
         <v>40</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>23</v>
@@ -3766,22 +3771,22 @@
     </row>
     <row r="42" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="D42" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="E42" t="s">
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>23</v>
@@ -3816,19 +3821,19 @@
     </row>
     <row r="43" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F43" t="s">
         <v>130</v>
@@ -3866,7 +3871,7 @@
     </row>
     <row r="44" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -3878,7 +3883,7 @@
         <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F44" t="s">
         <v>132</v>
@@ -3916,7 +3921,7 @@
     </row>
     <row r="45" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -3925,13 +3930,13 @@
         <v>133</v>
       </c>
       <c r="D45" t="s">
-        <v>134</v>
+        <v>37</v>
       </c>
       <c r="E45" t="s">
         <v>40</v>
       </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>37</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>23</v>
@@ -3966,22 +3971,22 @@
     </row>
     <row r="46" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
         <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>23</v>
@@ -4009,6 +4014,9 @@
       </c>
       <c r="O46" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="R46" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="X46" s="4" t="s">
         <v>31</v>
@@ -4016,25 +4024,25 @@
     </row>
     <row r="47" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="E47" t="s">
         <v>40</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>20</v>
@@ -4061,7 +4069,7 @@
         <v>29</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X47" s="4" t="s">
         <v>31</v>
@@ -4069,25 +4077,25 @@
     </row>
     <row r="48" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="D48" t="s">
         <v>136</v>
       </c>
       <c r="E48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F48" t="s">
         <v>136</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>20</v>
@@ -4114,7 +4122,7 @@
         <v>29</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X48" s="4" t="s">
         <v>31</v>
@@ -4122,7 +4130,7 @@
     </row>
     <row r="49" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -4137,7 +4145,7 @@
         <v>39</v>
       </c>
       <c r="F49" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>23</v>
@@ -4167,7 +4175,7 @@
         <v>29</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X49" s="4" t="s">
         <v>31</v>
@@ -4175,19 +4183,19 @@
     </row>
     <row r="50" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B50">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F50" t="s">
         <v>141</v>
@@ -4220,7 +4228,7 @@
         <v>29</v>
       </c>
       <c r="R50" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X50" s="4" t="s">
         <v>31</v>
@@ -4228,22 +4236,22 @@
     </row>
     <row r="51" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B51">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>23</v>
@@ -4273,7 +4281,7 @@
         <v>29</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X51" s="4" t="s">
         <v>31</v>
@@ -4281,22 +4289,22 @@
     </row>
     <row r="52" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="E52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>23</v>
@@ -4326,7 +4334,7 @@
         <v>29</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X52" s="4" t="s">
         <v>31</v>
@@ -4334,7 +4342,7 @@
     </row>
     <row r="53" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -4379,7 +4387,7 @@
         <v>29</v>
       </c>
       <c r="R53" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X53" s="4" t="s">
         <v>31</v>
@@ -4387,7 +4395,7 @@
     </row>
     <row r="54" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -4396,13 +4404,13 @@
         <v>146</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="F54" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>23</v>
@@ -4432,7 +4440,7 @@
         <v>29</v>
       </c>
       <c r="R54" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X54" s="4" t="s">
         <v>31</v>
@@ -4440,19 +4448,19 @@
     </row>
     <row r="55" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F55" t="s">
         <v>80</v>
@@ -4485,7 +4493,7 @@
         <v>29</v>
       </c>
       <c r="R55" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X55" s="4" t="s">
         <v>31</v>
@@ -4493,29 +4501,17 @@
     </row>
     <row r="56" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>125</v>
-      </c>
-      <c r="D56" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F56" t="s">
-        <v>82</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
       <c r="I56" s="4">
         <v>20040312</v>
       </c>
@@ -4538,7 +4534,7 @@
         <v>29</v>
       </c>
       <c r="R56" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X56" s="4" t="s">
         <v>31</v>
@@ -4546,17 +4542,29 @@
     </row>
     <row r="57" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
+        <v>129</v>
+      </c>
+      <c r="D57" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I57" s="4">
         <v>20040312</v>
       </c>
@@ -4579,7 +4587,7 @@
         <v>29</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="X57" s="4" t="s">
         <v>31</v>
@@ -4587,22 +4595,22 @@
     </row>
     <row r="58" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E58" t="s">
         <v>39</v>
       </c>
       <c r="F58" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>23</v>
@@ -4632,7 +4640,7 @@
         <v>29</v>
       </c>
       <c r="R58" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X58" s="4" t="s">
         <v>31</v>
@@ -4640,22 +4648,22 @@
     </row>
     <row r="59" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D59" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>23</v>
@@ -4684,8 +4692,8 @@
       <c r="O59" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R59" s="4" t="s">
-        <v>161</v>
+      <c r="W59" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="X59" s="4" t="s">
         <v>31</v>
@@ -4693,22 +4701,22 @@
     </row>
     <row r="60" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E60" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="F60" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>23</v>
@@ -4737,8 +4745,8 @@
       <c r="O60" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W60" s="4" t="s">
-        <v>162</v>
+      <c r="R60" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="X60" s="4" t="s">
         <v>31</v>
@@ -4746,22 +4754,22 @@
     </row>
     <row r="61" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E61" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F61" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>23</v>
@@ -4791,7 +4799,7 @@
         <v>29</v>
       </c>
       <c r="R61" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X61" s="4" t="s">
         <v>31</v>
@@ -4799,22 +4807,22 @@
     </row>
     <row r="62" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="B62">
+        <v>232</v>
+      </c>
+      <c r="B62" s="4">
         <v>3</v>
       </c>
-      <c r="C62" t="s">
-        <v>156</v>
-      </c>
-      <c r="D62" t="s">
-        <v>157</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="C62" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F62" t="s">
-        <v>157</v>
+      <c r="F62" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>23</v>
@@ -4844,7 +4852,7 @@
         <v>29</v>
       </c>
       <c r="R62" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X62" s="4" t="s">
         <v>31</v>
@@ -4852,22 +4860,22 @@
     </row>
     <row r="63" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B63" s="4">
         <v>3</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="E63" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>23</v>
@@ -4897,7 +4905,7 @@
         <v>29</v>
       </c>
       <c r="R63" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="X63" s="4" t="s">
         <v>31</v>
@@ -4905,25 +4913,25 @@
     </row>
     <row r="64" spans="1:24" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B64" s="4">
         <v>3</v>
       </c>
       <c r="C64" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>20</v>
@@ -4950,65 +4958,12 @@
         <v>29</v>
       </c>
       <c r="R64" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="V64" s="4">
+        <v>1</v>
       </c>
       <c r="X64" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B65" s="4">
-        <v>3</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I65" s="4">
-        <v>20040312</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M65" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N65" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R65" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="V65" s="4">
-        <v>1</v>
-      </c>
-      <c r="X65" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding how to denote coordinate uncertainty
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
+++ b/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E92CF0-EC30-D342-9027-A894AD92A5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94FF9F7-AA1A-084E-A1CF-C1FA0A36EF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15860" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19640" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{4C5623D5-05B7-E844-824D-79860B5E2E43}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{4C5623D5-05B7-E844-824D-79860B5E2E43}">
       <text>
         <r>
           <rPr>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="237">
   <si>
     <t>genus</t>
   </si>
@@ -1054,6 +1054,9 @@
   </si>
   <si>
     <t>in shade</t>
+  </si>
+  <si>
+    <t>coodUncM</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AB64"/>
+  <dimension ref="A1:AC64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1513,18 +1516,18 @@
     <col min="18" max="18" width="16.83203125" style="4" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" style="4" customWidth="1"/>
     <col min="20" max="20" width="8.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="4" customWidth="1"/>
-    <col min="23" max="23" width="13" style="4" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" style="4"/>
-    <col min="26" max="26" width="22.83203125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="16.5" style="4" customWidth="1"/>
-    <col min="28" max="28" width="70.6640625" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="4"/>
+    <col min="21" max="22" width="11.33203125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="16.5" style="4" customWidth="1"/>
+    <col min="24" max="24" width="13" style="4" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="10.83203125" style="4"/>
+    <col min="27" max="27" width="22.83203125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.5" style="4" customWidth="1"/>
+    <col min="29" max="29" width="70.6640625" style="4" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1589,28 +1592,31 @@
         <v>32</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>172</v>
       </c>
@@ -1657,17 +1663,18 @@
         <v>29</v>
       </c>
       <c r="U2"/>
-      <c r="W2" s="4" t="s">
+      <c r="V2"/>
+      <c r="X2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="Y2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>173</v>
       </c>
@@ -1714,17 +1721,18 @@
         <v>29</v>
       </c>
       <c r="U3"/>
-      <c r="W3" s="4" t="s">
+      <c r="V3"/>
+      <c r="X3" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="X3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="Y3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>174</v>
       </c>
@@ -1770,11 +1778,11 @@
       <c r="O4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>175</v>
       </c>
@@ -1820,14 +1828,14 @@
       <c r="O5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="Y5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>176</v>
       </c>
@@ -1873,14 +1881,14 @@
       <c r="O6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB6" t="s">
+      <c r="Y6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>177</v>
       </c>
@@ -1926,14 +1934,14 @@
       <c r="O7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB7" s="4" t="s">
+      <c r="Y7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC7" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>178</v>
       </c>
@@ -1979,12 +1987,12 @@
       <c r="O8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB8"/>
-    </row>
-    <row r="9" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC8"/>
+    </row>
+    <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>179</v>
       </c>
@@ -2030,14 +2038,14 @@
       <c r="O9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB9" t="s">
+      <c r="Y9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>180</v>
       </c>
@@ -2083,14 +2091,14 @@
       <c r="O10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB10" t="s">
+      <c r="Y10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>181</v>
       </c>
@@ -2139,14 +2147,14 @@
       <c r="R11" t="s">
         <v>92</v>
       </c>
-      <c r="X11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB11" t="s">
+      <c r="Y11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>182</v>
       </c>
@@ -2196,17 +2204,17 @@
       <c r="R12" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="X12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="X12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB12" t="s">
+      <c r="Y12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>183</v>
       </c>
@@ -2255,15 +2263,15 @@
       <c r="R13" t="s">
         <v>92</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>95</v>
       </c>
-      <c r="X13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB13"/>
-    </row>
-    <row r="14" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC13"/>
+    </row>
+    <row r="14" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>184</v>
       </c>
@@ -2312,14 +2320,14 @@
       <c r="R14" t="s">
         <v>92</v>
       </c>
-      <c r="X14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB14" t="s">
+      <c r="Y14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>185</v>
       </c>
@@ -2368,14 +2376,14 @@
       <c r="R15" t="s">
         <v>92</v>
       </c>
-      <c r="X15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB15" t="s">
+      <c r="Y15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>186</v>
       </c>
@@ -2424,14 +2432,14 @@
       <c r="R16" t="s">
         <v>92</v>
       </c>
-      <c r="X16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB16" t="s">
+      <c r="Y16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>187</v>
       </c>
@@ -2480,14 +2488,14 @@
       <c r="R17" t="s">
         <v>92</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB17" t="s">
+      <c r="Y17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>188</v>
       </c>
@@ -2536,14 +2544,14 @@
       <c r="R18" t="s">
         <v>92</v>
       </c>
-      <c r="X18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB18" t="s">
+      <c r="Y18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>189</v>
       </c>
@@ -2592,14 +2600,14 @@
       <c r="R19" t="s">
         <v>92</v>
       </c>
-      <c r="X19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB19" t="s">
+      <c r="Y19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>190</v>
       </c>
@@ -2648,14 +2656,14 @@
       <c r="R20" t="s">
         <v>92</v>
       </c>
-      <c r="X20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB20" t="s">
+      <c r="Y20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>191</v>
       </c>
@@ -2704,14 +2712,14 @@
       <c r="R21" t="s">
         <v>92</v>
       </c>
-      <c r="X21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB21" t="s">
+      <c r="Y21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>192</v>
       </c>
@@ -2760,14 +2768,14 @@
       <c r="R22" t="s">
         <v>92</v>
       </c>
-      <c r="X22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB22" t="s">
+      <c r="Y22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>193</v>
       </c>
@@ -2816,14 +2824,14 @@
       <c r="R23" t="s">
         <v>92</v>
       </c>
-      <c r="X23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB23" t="s">
+      <c r="Y23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>194</v>
       </c>
@@ -2872,14 +2880,14 @@
       <c r="R24" t="s">
         <v>93</v>
       </c>
-      <c r="X24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB24" t="s">
+      <c r="Y24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>195</v>
       </c>
@@ -2928,12 +2936,12 @@
       <c r="R25" t="s">
         <v>93</v>
       </c>
-      <c r="X25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB25"/>
-    </row>
-    <row r="26" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC25"/>
+    </row>
+    <row r="26" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>196</v>
       </c>
@@ -2982,14 +2990,14 @@
       <c r="R26" t="s">
         <v>94</v>
       </c>
-      <c r="X26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB26" t="s">
+      <c r="Y26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>197</v>
       </c>
@@ -3038,14 +3046,14 @@
       <c r="R27" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="X27" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB27" t="s">
+      <c r="Y27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>198</v>
       </c>
@@ -3094,14 +3102,14 @@
       <c r="R28" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="X28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB28" t="s">
+      <c r="Y28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>199</v>
       </c>
@@ -3150,11 +3158,11 @@
       <c r="R29" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="X29" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="51" x14ac:dyDescent="0.2">
+      <c r="Y29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>200</v>
       </c>
@@ -3203,14 +3211,14 @@
       <c r="R30" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="W30" s="4" t="s">
+      <c r="X30" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="X30" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y30" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>201</v>
       </c>
@@ -3256,11 +3264,11 @@
       <c r="O31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X31" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y31" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>202</v>
       </c>
@@ -3306,11 +3314,11 @@
       <c r="O32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X32" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>203</v>
       </c>
@@ -3359,11 +3367,11 @@
       <c r="R33" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="X33" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y33" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>204</v>
       </c>
@@ -3412,11 +3420,11 @@
       <c r="R34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="X34" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y34" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>205</v>
       </c>
@@ -3465,11 +3473,11 @@
       <c r="R35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="X35" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y35" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>206</v>
       </c>
@@ -3515,11 +3523,11 @@
       <c r="O36" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X36" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y36" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>207</v>
       </c>
@@ -3565,11 +3573,11 @@
       <c r="O37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X37" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y37" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>208</v>
       </c>
@@ -3615,11 +3623,11 @@
       <c r="O38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X38" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y38" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>209</v>
       </c>
@@ -3665,11 +3673,11 @@
       <c r="O39" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X39" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y39" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>210</v>
       </c>
@@ -3715,11 +3723,11 @@
       <c r="O40" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X40" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y40" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>211</v>
       </c>
@@ -3765,11 +3773,11 @@
       <c r="O41" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X41" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y41" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>212</v>
       </c>
@@ -3815,11 +3823,11 @@
       <c r="O42" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X42" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y42" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>213</v>
       </c>
@@ -3865,11 +3873,11 @@
       <c r="O43" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X43" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y43" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>214</v>
       </c>
@@ -3915,11 +3923,11 @@
       <c r="O44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X44" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y44" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>215</v>
       </c>
@@ -3965,11 +3973,11 @@
       <c r="O45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X45" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y45" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>216</v>
       </c>
@@ -4018,11 +4026,11 @@
       <c r="R46" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="X46" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y46" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>217</v>
       </c>
@@ -4071,11 +4079,11 @@
       <c r="R47" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X47" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y47" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>218</v>
       </c>
@@ -4124,11 +4132,11 @@
       <c r="R48" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X48" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y48" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>219</v>
       </c>
@@ -4177,11 +4185,11 @@
       <c r="R49" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X49" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y49" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>220</v>
       </c>
@@ -4230,11 +4238,11 @@
       <c r="R50" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X50" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y50" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>221</v>
       </c>
@@ -4283,11 +4291,11 @@
       <c r="R51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X51" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y51" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>222</v>
       </c>
@@ -4336,11 +4344,11 @@
       <c r="R52" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X52" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y52" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>223</v>
       </c>
@@ -4389,11 +4397,11 @@
       <c r="R53" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X53" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y53" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>224</v>
       </c>
@@ -4442,11 +4450,11 @@
       <c r="R54" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X54" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y54" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>225</v>
       </c>
@@ -4495,11 +4503,11 @@
       <c r="R55" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X55" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y55" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>226</v>
       </c>
@@ -4536,11 +4544,11 @@
       <c r="R56" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X56" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y56" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>227</v>
       </c>
@@ -4589,11 +4597,11 @@
       <c r="R57" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="X57" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y57" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>228</v>
       </c>
@@ -4642,11 +4650,11 @@
       <c r="R58" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="X58" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y58" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>229</v>
       </c>
@@ -4692,14 +4700,14 @@
       <c r="O59" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W59" s="4" t="s">
+      <c r="X59" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="X59" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y59" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>230</v>
       </c>
@@ -4748,11 +4756,11 @@
       <c r="R60" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="X60" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y60" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>231</v>
       </c>
@@ -4801,11 +4809,11 @@
       <c r="R61" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="X61" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y61" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>232</v>
       </c>
@@ -4854,11 +4862,11 @@
       <c r="R62" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="X62" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y62" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>233</v>
       </c>
@@ -4907,11 +4915,11 @@
       <c r="R63" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="X63" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y63" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>234</v>
       </c>
@@ -4960,10 +4968,10 @@
       <c r="R64" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="V64" s="4">
+      <c r="W64" s="4">
         <v>1</v>
       </c>
-      <c r="X64" s="4" t="s">
+      <c r="Y64" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added gbif taxonomy checker
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
+++ b/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94FF9F7-AA1A-084E-A1CF-C1FA0A36EF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8FD4F9-2E6D-004F-AD02-23AE34C14387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19640" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -594,9 +594,6 @@
     <t>Cama lei</t>
   </si>
   <si>
-    <t>Camassa leichtlinii</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -855,12 +852,6 @@
     <t>Plec con</t>
   </si>
   <si>
-    <t>Rumeace</t>
-  </si>
-  <si>
-    <t>Rumiaceae</t>
-  </si>
-  <si>
     <t>tribe</t>
   </si>
   <si>
@@ -1056,7 +1047,16 @@
     <t>in shade</t>
   </si>
   <si>
-    <t>coodUncM</t>
+    <t>vCoodUncM</t>
+  </si>
+  <si>
+    <t>Rumex</t>
+  </si>
+  <si>
+    <t>Rume ace</t>
+  </si>
+  <si>
+    <t>Camassia leichtlinii</t>
   </si>
 </sst>
 </file>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,7 +1532,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>58</v>
@@ -1592,7 +1592,7 @@
         <v>32</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>16</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1723,7 +1723,7 @@
       <c r="U3"/>
       <c r="V3"/>
       <c r="X3" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="Y3" s="4" t="s">
         <v>31</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="10" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="11" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2145,7 +2145,7 @@
         <v>29</v>
       </c>
       <c r="R11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y11" s="4" t="s">
         <v>31</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="12" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2202,10 +2202,10 @@
       </c>
       <c r="P12"/>
       <c r="R12" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y12" s="4" t="s">
         <v>31</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2261,10 +2261,10 @@
         <v>29</v>
       </c>
       <c r="R13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y13" s="4" t="s">
         <v>31</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="14" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2318,7 +2318,7 @@
         <v>29</v>
       </c>
       <c r="R14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y14" s="4" t="s">
         <v>31</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="15" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2374,7 +2374,7 @@
         <v>29</v>
       </c>
       <c r="R15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y15" s="4" t="s">
         <v>31</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="16" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2430,7 +2430,7 @@
         <v>29</v>
       </c>
       <c r="R16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y16" s="4" t="s">
         <v>31</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="17" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2486,7 +2486,7 @@
         <v>29</v>
       </c>
       <c r="R17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y17" s="4" t="s">
         <v>31</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="18" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2542,7 +2542,7 @@
         <v>29</v>
       </c>
       <c r="R18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y18" s="4" t="s">
         <v>31</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="19" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2598,7 +2598,7 @@
         <v>29</v>
       </c>
       <c r="R19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y19" s="4" t="s">
         <v>31</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="20" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2654,7 +2654,7 @@
         <v>29</v>
       </c>
       <c r="R20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y20" s="4" t="s">
         <v>31</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="21" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2710,7 +2710,7 @@
         <v>29</v>
       </c>
       <c r="R21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y21" s="4" t="s">
         <v>31</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="22" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2766,7 +2766,7 @@
         <v>29</v>
       </c>
       <c r="R22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y22" s="4" t="s">
         <v>31</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="23" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2822,7 +2822,7 @@
         <v>29</v>
       </c>
       <c r="R23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y23" s="4" t="s">
         <v>31</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="24" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2842,13 +2842,13 @@
         <v>81</v>
       </c>
       <c r="D24" t="s">
+        <v>236</v>
+      </c>
+      <c r="E24" t="s">
         <v>82</v>
       </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>236</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>23</v>
@@ -2878,7 +2878,7 @@
         <v>29</v>
       </c>
       <c r="R24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y24" s="4" t="s">
         <v>31</v>
@@ -2889,22 +2889,22 @@
     </row>
     <row r="25" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
@@ -2934,7 +2934,7 @@
         <v>29</v>
       </c>
       <c r="R25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y25" s="4" t="s">
         <v>31</v>
@@ -2943,22 +2943,22 @@
     </row>
     <row r="26" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
         <v>84</v>
       </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>23</v>
@@ -2988,7 +2988,7 @@
         <v>29</v>
       </c>
       <c r="R26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y26" s="4" t="s">
         <v>31</v>
@@ -2999,22 +2999,22 @@
     </row>
     <row r="27" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
         <v>86</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>23</v>
@@ -3044,7 +3044,7 @@
         <v>29</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y27" s="4" t="s">
         <v>31</v>
@@ -3055,22 +3055,22 @@
     </row>
     <row r="28" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
         <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
       </c>
       <c r="E28" t="s">
         <v>39</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>23</v>
@@ -3100,7 +3100,7 @@
         <v>29</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y28" s="4" t="s">
         <v>31</v>
@@ -3111,22 +3111,22 @@
     </row>
     <row r="29" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E29" t="s">
         <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
@@ -3156,7 +3156,7 @@
         <v>29</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y29" s="4" t="s">
         <v>31</v>
@@ -3164,22 +3164,22 @@
     </row>
     <row r="30" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
@@ -3209,10 +3209,10 @@
         <v>29</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X30" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y30" s="4" t="s">
         <v>31</v>
@@ -3220,22 +3220,22 @@
     </row>
     <row r="31" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
@@ -3270,22 +3270,22 @@
     </row>
     <row r="32" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>0</v>
@@ -3320,22 +3320,22 @@
     </row>
     <row r="33" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>23</v>
@@ -3365,7 +3365,7 @@
         <v>29</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y33" s="4" t="s">
         <v>31</v>
@@ -3373,22 +3373,22 @@
     </row>
     <row r="34" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>0</v>
@@ -3418,7 +3418,7 @@
         <v>29</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y34" s="4" t="s">
         <v>31</v>
@@ -3426,26 +3426,26 @@
     </row>
     <row r="35" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="H35" s="4" t="s">
         <v>20</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>29</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y35" s="4" t="s">
         <v>31</v>
@@ -3479,22 +3479,22 @@
     </row>
     <row r="36" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
         <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
       </c>
       <c r="E36" t="s">
         <v>40</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>23</v>
@@ -3529,22 +3529,22 @@
     </row>
     <row r="37" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
       <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" t="s">
         <v>119</v>
-      </c>
-      <c r="D37" t="s">
-        <v>120</v>
       </c>
       <c r="E37" t="s">
         <v>40</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>23</v>
@@ -3579,22 +3579,22 @@
     </row>
     <row r="38" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" t="s">
         <v>121</v>
-      </c>
-      <c r="D38" t="s">
-        <v>122</v>
       </c>
       <c r="E38" t="s">
         <v>40</v>
       </c>
       <c r="F38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>23</v>
@@ -3629,13 +3629,13 @@
     </row>
     <row r="39" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
@@ -3679,22 +3679,22 @@
     </row>
     <row r="40" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
       <c r="C40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" t="s">
         <v>124</v>
-      </c>
-      <c r="D40" t="s">
-        <v>125</v>
       </c>
       <c r="E40" t="s">
         <v>40</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>23</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="41" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -3779,22 +3779,22 @@
     </row>
     <row r="42" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
         <v>126</v>
-      </c>
-      <c r="D42" t="s">
-        <v>127</v>
       </c>
       <c r="E42" t="s">
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>23</v>
@@ -3829,22 +3829,22 @@
     </row>
     <row r="43" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
       <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
         <v>129</v>
-      </c>
-      <c r="D43" t="s">
-        <v>130</v>
       </c>
       <c r="E43" t="s">
         <v>39</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>23</v>
@@ -3879,22 +3879,22 @@
     </row>
     <row r="44" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
       <c r="C44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" t="s">
         <v>131</v>
-      </c>
-      <c r="D44" t="s">
-        <v>132</v>
       </c>
       <c r="E44" t="s">
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>23</v>
@@ -3929,13 +3929,13 @@
     </row>
     <row r="45" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
         <v>37</v>
@@ -3979,7 +3979,7 @@
     </row>
     <row r="46" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -4024,7 +4024,7 @@
         <v>29</v>
       </c>
       <c r="R46" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y46" s="4" t="s">
         <v>31</v>
@@ -4032,22 +4032,22 @@
     </row>
     <row r="47" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
         <v>40</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>0</v>
@@ -4077,7 +4077,7 @@
         <v>29</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y47" s="4" t="s">
         <v>31</v>
@@ -4085,22 +4085,22 @@
     </row>
     <row r="48" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" t="s">
         <v>135</v>
-      </c>
-      <c r="D48" t="s">
-        <v>136</v>
       </c>
       <c r="E48" t="s">
         <v>39</v>
       </c>
       <c r="F48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>23</v>
@@ -4130,7 +4130,7 @@
         <v>29</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y48" s="4" t="s">
         <v>31</v>
@@ -4138,22 +4138,22 @@
     </row>
     <row r="49" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B49">
         <v>3</v>
       </c>
       <c r="C49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" t="s">
         <v>137</v>
-      </c>
-      <c r="D49" t="s">
-        <v>138</v>
       </c>
       <c r="E49" t="s">
         <v>39</v>
       </c>
       <c r="F49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>23</v>
@@ -4183,7 +4183,7 @@
         <v>29</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y49" s="4" t="s">
         <v>31</v>
@@ -4191,22 +4191,22 @@
     </row>
     <row r="50" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B50">
         <v>3</v>
       </c>
       <c r="C50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" t="s">
         <v>140</v>
-      </c>
-      <c r="D50" t="s">
-        <v>141</v>
       </c>
       <c r="E50" t="s">
         <v>40</v>
       </c>
       <c r="F50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>23</v>
@@ -4236,7 +4236,7 @@
         <v>29</v>
       </c>
       <c r="R50" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y50" s="4" t="s">
         <v>31</v>
@@ -4244,7 +4244,7 @@
     </row>
     <row r="51" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -4289,7 +4289,7 @@
         <v>29</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y51" s="4" t="s">
         <v>31</v>
@@ -4297,22 +4297,22 @@
     </row>
     <row r="52" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" t="s">
         <v>142</v>
-      </c>
-      <c r="D52" t="s">
-        <v>143</v>
       </c>
       <c r="E52" t="s">
         <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>23</v>
@@ -4342,7 +4342,7 @@
         <v>29</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y52" s="4" t="s">
         <v>31</v>
@@ -4350,22 +4350,22 @@
     </row>
     <row r="53" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B53">
         <v>3</v>
       </c>
       <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" t="s">
         <v>144</v>
-      </c>
-      <c r="D53" t="s">
-        <v>145</v>
       </c>
       <c r="E53" t="s">
         <v>40</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>23</v>
@@ -4395,7 +4395,7 @@
         <v>29</v>
       </c>
       <c r="R53" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y53" s="4" t="s">
         <v>31</v>
@@ -4403,19 +4403,19 @@
     </row>
     <row r="54" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
         <v>77</v>
       </c>
       <c r="E54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F54" t="s">
         <v>78</v>
@@ -4448,7 +4448,7 @@
         <v>29</v>
       </c>
       <c r="R54" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y54" s="4" t="s">
         <v>31</v>
@@ -4456,13 +4456,13 @@
     </row>
     <row r="55" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D55" t="s">
         <v>80</v>
@@ -4501,7 +4501,7 @@
         <v>29</v>
       </c>
       <c r="R55" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y55" s="4" t="s">
         <v>31</v>
@@ -4509,13 +4509,13 @@
     </row>
     <row r="56" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D56"/>
       <c r="E56"/>
@@ -4542,7 +4542,7 @@
         <v>29</v>
       </c>
       <c r="R56" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y56" s="4" t="s">
         <v>31</v>
@@ -4550,22 +4550,22 @@
     </row>
     <row r="57" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
       <c r="C57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" t="s">
         <v>129</v>
-      </c>
-      <c r="D57" t="s">
-        <v>130</v>
       </c>
       <c r="E57" t="s">
         <v>39</v>
       </c>
       <c r="F57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>23</v>
@@ -4595,7 +4595,7 @@
         <v>29</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y57" s="4" t="s">
         <v>31</v>
@@ -4603,22 +4603,22 @@
     </row>
     <row r="58" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" t="s">
         <v>148</v>
-      </c>
-      <c r="D58" t="s">
-        <v>149</v>
       </c>
       <c r="E58" t="s">
         <v>39</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>23</v>
@@ -4648,7 +4648,7 @@
         <v>29</v>
       </c>
       <c r="R58" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Y58" s="4" t="s">
         <v>31</v>
@@ -4656,22 +4656,22 @@
     </row>
     <row r="59" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" t="s">
         <v>151</v>
-      </c>
-      <c r="D59" t="s">
-        <v>152</v>
       </c>
       <c r="E59" t="s">
         <v>65</v>
       </c>
       <c r="F59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>23</v>
@@ -4701,7 +4701,7 @@
         <v>29</v>
       </c>
       <c r="X59" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y59" s="4" t="s">
         <v>31</v>
@@ -4709,22 +4709,22 @@
     </row>
     <row r="60" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" t="s">
         <v>162</v>
-      </c>
-      <c r="D60" t="s">
-        <v>163</v>
       </c>
       <c r="E60" t="s">
         <v>39</v>
       </c>
       <c r="F60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>23</v>
@@ -4754,7 +4754,7 @@
         <v>29</v>
       </c>
       <c r="R60" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y60" s="4" t="s">
         <v>31</v>
@@ -4762,22 +4762,22 @@
     </row>
     <row r="61" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" t="s">
         <v>154</v>
-      </c>
-      <c r="D61" t="s">
-        <v>155</v>
       </c>
       <c r="E61" t="s">
         <v>40</v>
       </c>
       <c r="F61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>23</v>
@@ -4807,7 +4807,7 @@
         <v>29</v>
       </c>
       <c r="R61" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y61" s="4" t="s">
         <v>31</v>
@@ -4815,22 +4815,22 @@
     </row>
     <row r="62" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B62" s="4">
         <v>3</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>23</v>
@@ -4860,7 +4860,7 @@
         <v>29</v>
       </c>
       <c r="R62" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Y62" s="4" t="s">
         <v>31</v>
@@ -4868,22 +4868,22 @@
     </row>
     <row r="63" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B63" s="4">
         <v>3</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>23</v>
@@ -4913,7 +4913,7 @@
         <v>29</v>
       </c>
       <c r="R63" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Y63" s="4" t="s">
         <v>31</v>
@@ -4921,25 +4921,25 @@
     </row>
     <row r="64" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B64" s="4">
         <v>3</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>169</v>
+        <v>235</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>20</v>
@@ -4966,7 +4966,7 @@
         <v>29</v>
       </c>
       <c r="R64" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W64" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
beginning to enter HJ8 to test template
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
+++ b/data/digitized_data/HJ-occ-entry-template_22-11-11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE000EC-1EBA-CE4B-843A-2974CDDE977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBBF635-6525-1A44-A87A-F919EEE70CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1900" windowWidth="28140" windowHeight="16880" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="254">
   <si>
     <t>genus</t>
   </si>
@@ -771,9 +771,6 @@
     <t>Mimul gut</t>
   </si>
   <si>
-    <t>ortar gramino</t>
-  </si>
-  <si>
     <t>Orob uni</t>
   </si>
   <si>
@@ -895,13 +892,229 @@
   </si>
   <si>
     <t>Clarkia amoena Torilis japonica</t>
+  </si>
+  <si>
+    <t>HJ-8</t>
+  </si>
+  <si>
+    <t>Elodea densa</t>
+  </si>
+  <si>
+    <t>Egeria densa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species </t>
+  </si>
+  <si>
+    <t>Metchosin</t>
+  </si>
+  <si>
+    <t>Vancouver Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoreline of lake </t>
+  </si>
+  <si>
+    <t>south shore of Matheson Lake, Metchosin</t>
+  </si>
+  <si>
+    <t>Potamogeton richardsonii</t>
+  </si>
+  <si>
+    <t>P praelongus</t>
+  </si>
+  <si>
+    <t>Potamogeton praelongus</t>
+  </si>
+  <si>
+    <t>Carex excissata</t>
+  </si>
+  <si>
+    <t>Carex exsiccata</t>
+  </si>
+  <si>
+    <t>C. obnupta</t>
+  </si>
+  <si>
+    <t>Carex obnupta</t>
+  </si>
+  <si>
+    <t>Agrostis gigatea</t>
+  </si>
+  <si>
+    <t>Agrostis gigantea</t>
+  </si>
+  <si>
+    <t>Calieagon gig</t>
+  </si>
+  <si>
+    <t>Nuphar polysepala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penninsula middle of south site, Matheson Lake, Metchosin </t>
+  </si>
+  <si>
+    <t>Spiraea douglassii</t>
+  </si>
+  <si>
+    <t>Salix lasiadra</t>
+  </si>
+  <si>
+    <t>Salix lasiandra</t>
+  </si>
+  <si>
+    <t>Sparganium emersum</t>
+  </si>
+  <si>
+    <t>Lemna minor</t>
+  </si>
+  <si>
+    <t>Typha latifolia</t>
+  </si>
+  <si>
+    <t>Myriopphyllum spicatum</t>
+  </si>
+  <si>
+    <t>west end of Matheson Lake, Metchosin</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>Rubus spectabilis</t>
+  </si>
+  <si>
+    <t>Lycopus uniflorus</t>
+  </si>
+  <si>
+    <t>Veronica americana</t>
+  </si>
+  <si>
+    <t>Aster subspicatum</t>
+  </si>
+  <si>
+    <t>Symphyotricum subspicatum</t>
+  </si>
+  <si>
+    <t>north side of Matheson Lake, Metchosin</t>
+  </si>
+  <si>
+    <t>Carex lasiocarpa</t>
+  </si>
+  <si>
+    <t>Scirpus acutus</t>
+  </si>
+  <si>
+    <t>two large beds</t>
+  </si>
+  <si>
+    <t>Potamogeton robbinsii</t>
+  </si>
+  <si>
+    <t>Potamogeton amplifolius</t>
+  </si>
+  <si>
+    <t>Isoetes echinospora</t>
+  </si>
+  <si>
+    <t>behind Scirpus beds</t>
+  </si>
+  <si>
+    <t>Eleocharis palustris</t>
+  </si>
+  <si>
+    <t>Utricularia vulgaris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on log, shoreline of lake </t>
+  </si>
+  <si>
+    <t>Carex cusickii</t>
+  </si>
+  <si>
+    <t>Potentilla palustris</t>
+  </si>
+  <si>
+    <t>Comarum palustre</t>
+  </si>
+  <si>
+    <t>Potamogeton natans</t>
+  </si>
+  <si>
+    <t>Drosera rotundifolia</t>
+  </si>
+  <si>
+    <t>Blinkhorn Lake, Metchosin</t>
+  </si>
+  <si>
+    <t>approx 30% lake cover with Nuphar polysepala</t>
+  </si>
+  <si>
+    <t>Nymphae odorata</t>
+  </si>
+  <si>
+    <t>Nymphae sp. odorata</t>
+  </si>
+  <si>
+    <t>approx 30% lake cover with Nymphae odorata</t>
+  </si>
+  <si>
+    <t>aquatic in lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edges of lake </t>
+  </si>
+  <si>
+    <t>Schoenoplectus acutus</t>
+  </si>
+  <si>
+    <t>Spiraea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salix </t>
+  </si>
+  <si>
+    <t>Alder</t>
+  </si>
+  <si>
+    <t>Alnus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h </t>
+  </si>
+  <si>
+    <t>Agrostis scabra</t>
+  </si>
+  <si>
+    <t>Sphagnum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Sphagnum mats in lake </t>
+  </si>
+  <si>
+    <t>Saltspring Island</t>
+  </si>
+  <si>
+    <t>in lake</t>
+  </si>
+  <si>
+    <t>6 km lake, Saltspring Island</t>
+  </si>
+  <si>
+    <t>mostly open water in lake with Sphagnum mats</t>
+  </si>
+  <si>
+    <t>Carex oederi</t>
+  </si>
+  <si>
+    <t>Carex interior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -955,6 +1168,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1019,7 +1239,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,10 +1557,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AD65"/>
+  <dimension ref="A1:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1357,7 +1581,7 @@
     <col min="13" max="13" width="16.83203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="20.33203125" style="4" customWidth="1"/>
     <col min="15" max="15" width="21.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="4"/>
+    <col min="16" max="16" width="13.33203125" style="4" customWidth="1"/>
     <col min="17" max="17" width="22.1640625" style="4" customWidth="1"/>
     <col min="18" max="18" width="8.5" style="4" customWidth="1"/>
     <col min="19" max="19" width="16.83203125" style="4" customWidth="1"/>
@@ -1370,20 +1594,20 @@
     <col min="26" max="26" width="14.6640625" style="4" customWidth="1"/>
     <col min="27" max="27" width="10.83203125" style="4"/>
     <col min="28" max="28" width="14.33203125" style="4" customWidth="1"/>
-    <col min="29" max="29" width="28.5" style="4" customWidth="1"/>
+    <col min="29" max="29" width="23.6640625" style="4" customWidth="1"/>
     <col min="30" max="30" width="70.6640625" style="4" customWidth="1"/>
     <col min="31" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>54</v>
@@ -1410,13 +1634,13 @@
         <v>4</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>2</v>
@@ -1443,7 +1667,7 @@
         <v>28</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>12</v>
@@ -1469,7 +1693,7 @@
     </row>
     <row r="2" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1517,7 +1741,7 @@
         <v>25</v>
       </c>
       <c r="V2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W2"/>
       <c r="Y2" s="4" t="s">
@@ -1527,7 +1751,7 @@
         <v>27</v>
       </c>
       <c r="AC2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD2" t="s">
         <v>37</v>
@@ -1535,7 +1759,7 @@
     </row>
     <row r="3" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1583,11 +1807,11 @@
         <v>25</v>
       </c>
       <c r="V3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W3"/>
       <c r="Y3" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z3" s="4" t="s">
         <v>27</v>
@@ -1598,7 +1822,7 @@
     </row>
     <row r="4" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1651,7 +1875,7 @@
     </row>
     <row r="5" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1699,7 +1923,7 @@
         <v>25</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>27</v>
@@ -1710,7 +1934,7 @@
     </row>
     <row r="6" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1758,7 +1982,7 @@
         <v>25</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>27</v>
@@ -1769,7 +1993,7 @@
     </row>
     <row r="7" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1825,7 +2049,7 @@
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1873,7 +2097,7 @@
         <v>25</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>27</v>
@@ -1882,7 +2106,7 @@
     </row>
     <row r="9" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1938,7 +2162,7 @@
     </row>
     <row r="10" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1986,7 +2210,7 @@
         <v>25</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>27</v>
@@ -1997,7 +2221,7 @@
     </row>
     <row r="11" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2056,7 +2280,7 @@
     </row>
     <row r="12" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2119,7 +2343,7 @@
     </row>
     <row r="13" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2179,7 +2403,7 @@
     </row>
     <row r="14" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2238,7 +2462,7 @@
     </row>
     <row r="15" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2297,7 +2521,7 @@
     </row>
     <row r="16" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2356,7 +2580,7 @@
     </row>
     <row r="17" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2415,7 +2639,7 @@
     </row>
     <row r="18" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2474,7 +2698,7 @@
     </row>
     <row r="19" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -2533,7 +2757,7 @@
     </row>
     <row r="20" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2592,7 +2816,7 @@
     </row>
     <row r="21" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2651,7 +2875,7 @@
     </row>
     <row r="22" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -2710,7 +2934,7 @@
     </row>
     <row r="23" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2769,7 +2993,7 @@
     </row>
     <row r="24" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2781,13 +3005,13 @@
         <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F24" t="s">
         <v>78</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>19</v>
@@ -2828,7 +3052,7 @@
     </row>
     <row r="25" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2885,7 +3109,7 @@
     </row>
     <row r="26" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -2944,7 +3168,7 @@
     </row>
     <row r="27" spans="1:30" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -2953,14 +3177,14 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27"/>
+      <c r="G27" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>19</v>
@@ -2991,7 +3215,7 @@
       </c>
       <c r="S27"/>
       <c r="Y27" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z27" s="4" t="s">
         <v>27</v>
@@ -3000,7 +3224,7 @@
     </row>
     <row r="28" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -3059,7 +3283,7 @@
     </row>
     <row r="29" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -3118,7 +3342,7 @@
     </row>
     <row r="30" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -3174,7 +3398,7 @@
     </row>
     <row r="31" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -3233,7 +3457,7 @@
     </row>
     <row r="32" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -3286,7 +3510,7 @@
     </row>
     <row r="33" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -3339,7 +3563,7 @@
     </row>
     <row r="34" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -3395,7 +3619,7 @@
     </row>
     <row r="35" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -3451,7 +3675,7 @@
     </row>
     <row r="36" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -3507,7 +3731,7 @@
     </row>
     <row r="37" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -3560,7 +3784,7 @@
     </row>
     <row r="38" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -3613,7 +3837,7 @@
     </row>
     <row r="39" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -3666,7 +3890,7 @@
     </row>
     <row r="40" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -3719,7 +3943,7 @@
     </row>
     <row r="41" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -3772,7 +3996,7 @@
     </row>
     <row r="42" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -3825,7 +4049,7 @@
     </row>
     <row r="43" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -3878,7 +4102,7 @@
     </row>
     <row r="44" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -3931,7 +4155,7 @@
     </row>
     <row r="45" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -3984,7 +4208,7 @@
     </row>
     <row r="46" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -4037,7 +4261,7 @@
     </row>
     <row r="47" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -4085,7 +4309,7 @@
         <v>25</v>
       </c>
       <c r="S47" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Z47" s="4" t="s">
         <v>27</v>
@@ -4093,7 +4317,7 @@
     </row>
     <row r="48" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -4102,7 +4326,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E48" t="s">
         <v>128</v>
@@ -4141,7 +4365,7 @@
         <v>25</v>
       </c>
       <c r="S48" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z48" s="4" t="s">
         <v>27</v>
@@ -4149,7 +4373,7 @@
     </row>
     <row r="49" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -4197,7 +4421,7 @@
         <v>25</v>
       </c>
       <c r="S49" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z49" s="4" t="s">
         <v>27</v>
@@ -4205,7 +4429,7 @@
     </row>
     <row r="50" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -4253,7 +4477,7 @@
         <v>25</v>
       </c>
       <c r="S50" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z50" s="4" t="s">
         <v>27</v>
@@ -4261,7 +4485,7 @@
     </row>
     <row r="51" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -4309,7 +4533,7 @@
         <v>25</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z51" s="4" t="s">
         <v>27</v>
@@ -4317,7 +4541,7 @@
     </row>
     <row r="52" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -4365,7 +4589,7 @@
         <v>25</v>
       </c>
       <c r="S52" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z52" s="4" t="s">
         <v>27</v>
@@ -4373,7 +4597,7 @@
     </row>
     <row r="53" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -4421,7 +4645,7 @@
         <v>25</v>
       </c>
       <c r="S53" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z53" s="4" t="s">
         <v>27</v>
@@ -4429,7 +4653,7 @@
     </row>
     <row r="54" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -4477,7 +4701,7 @@
         <v>25</v>
       </c>
       <c r="S54" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z54" s="4" t="s">
         <v>27</v>
@@ -4485,7 +4709,7 @@
     </row>
     <row r="55" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -4533,7 +4757,7 @@
         <v>25</v>
       </c>
       <c r="S55" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z55" s="4" t="s">
         <v>27</v>
@@ -4541,7 +4765,7 @@
     </row>
     <row r="56" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -4589,7 +4813,7 @@
         <v>25</v>
       </c>
       <c r="S56" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z56" s="4" t="s">
         <v>27</v>
@@ -4597,20 +4821,32 @@
     </row>
     <row r="57" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
       <c r="C57">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
-      </c>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
+        <v>123</v>
+      </c>
+      <c r="E57" t="s">
+        <v>124</v>
+      </c>
+      <c r="F57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" t="s">
+        <v>124</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="J57" s="4">
         <v>20040312</v>
       </c>
@@ -4633,7 +4869,7 @@
         <v>25</v>
       </c>
       <c r="S57" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z57" s="4" t="s">
         <v>27</v>
@@ -4641,25 +4877,25 @@
     </row>
     <row r="58" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="C58">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E58" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="F58" t="s">
         <v>35</v>
       </c>
       <c r="G58" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>19</v>
@@ -4697,25 +4933,25 @@
     </row>
     <row r="59" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E59" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F59" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="G59" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>19</v>
@@ -4744,7 +4980,7 @@
       <c r="P59" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S59" s="4" t="s">
+      <c r="Y59" s="4" t="s">
         <v>153</v>
       </c>
       <c r="Z59" s="4" t="s">
@@ -4753,25 +4989,25 @@
     </row>
     <row r="60" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
       <c r="C60">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D60" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E60" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F60" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="G60" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>19</v>
@@ -4800,7 +5036,7 @@
       <c r="P60" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Y60" s="4" t="s">
+      <c r="S60" s="4" t="s">
         <v>154</v>
       </c>
       <c r="Z60" s="4" t="s">
@@ -4809,25 +5045,25 @@
     </row>
     <row r="61" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B61">
         <v>3</v>
       </c>
       <c r="C61">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D61" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E61" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F61" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G61" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>19</v>
@@ -4857,33 +5093,33 @@
         <v>25</v>
       </c>
       <c r="S61" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z61" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62">
+        <v>178</v>
+      </c>
+      <c r="B62" s="4">
         <v>3</v>
       </c>
       <c r="C62">
-        <v>27</v>
-      </c>
-      <c r="D62" t="s">
-        <v>148</v>
-      </c>
-      <c r="E62" t="s">
-        <v>149</v>
-      </c>
-      <c r="F62" t="s">
-        <v>36</v>
-      </c>
-      <c r="G62" t="s">
-        <v>149</v>
+        <v>28</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>19</v>
@@ -4913,7 +5149,7 @@
         <v>25</v>
       </c>
       <c r="S62" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Z62" s="4" t="s">
         <v>27</v>
@@ -4921,22 +5157,22 @@
     </row>
     <row r="63" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="4">
         <v>3</v>
       </c>
       <c r="C63">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>160</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>160</v>
@@ -4969,7 +5205,7 @@
         <v>25</v>
       </c>
       <c r="S63" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z63" s="4" t="s">
         <v>27</v>
@@ -4977,28 +5213,28 @@
     </row>
     <row r="64" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B64" s="4">
         <v>3</v>
       </c>
       <c r="C64">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>16</v>
@@ -5025,68 +5261,2510 @@
         <v>25</v>
       </c>
       <c r="S64" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+      <c r="X64" s="4">
+        <v>1</v>
       </c>
       <c r="Z64" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J65" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P65" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q65" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z65" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB65" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC65" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B66" s="4">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4">
+        <v>2</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K66" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P66" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q66" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z66" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB66" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC66" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+      <c r="C67" s="4">
         <v>3</v>
       </c>
-      <c r="C65">
-        <v>30</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F65" s="4" t="s">
+      <c r="D67" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J67" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P67" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q67" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z67" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB67" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC67" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1</v>
+      </c>
+      <c r="C68" s="4">
+        <v>4</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J68" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z68" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC68" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="4">
+        <v>1</v>
+      </c>
+      <c r="C69" s="4">
+        <v>5</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P69" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q69" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z69" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC69" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
+      </c>
+      <c r="C70" s="4">
+        <v>6</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P70" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q70" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z70" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB70" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC70" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="C71" s="4">
+        <v>7</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M71" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P71" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q71" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z71" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB71" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC71" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1</v>
+      </c>
+      <c r="C72" s="4">
+        <v>8</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P72" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q72" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z72" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB72" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC72" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73" s="4">
+        <v>1</v>
+      </c>
+      <c r="C73" s="4">
+        <v>9</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J73" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P73" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q73" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z73" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B74" s="4">
+        <v>1</v>
+      </c>
+      <c r="C74" s="4">
+        <v>10</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N74" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P74" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q74" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z74" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" s="4">
+        <v>1</v>
+      </c>
+      <c r="C75" s="4">
+        <v>11</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G65" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J65" s="4">
-        <v>20040312</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M65" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N65" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P65" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S65" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="X65" s="4">
+      <c r="G75" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q75" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z75" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" s="4">
         <v>1</v>
       </c>
-      <c r="Z65" s="4" t="s">
+      <c r="C76" s="4">
+        <v>12</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J76" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N76" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q76" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z76" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" s="4">
+        <v>1</v>
+      </c>
+      <c r="C77" s="4">
+        <v>13</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J77" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q77" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z77" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="C78" s="4">
+        <v>14</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N78" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P78" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q78" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z78" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B79" s="4">
+        <v>1</v>
+      </c>
+      <c r="C79" s="4">
+        <v>15</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J79" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y79" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z79" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B80" s="4">
+        <v>1</v>
+      </c>
+      <c r="C80" s="4">
+        <v>16</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N80" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y80" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z80" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="4">
+        <v>1</v>
+      </c>
+      <c r="C81" s="4">
+        <v>17</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y81" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z81" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="4">
+        <v>1</v>
+      </c>
+      <c r="C82" s="4">
+        <v>18</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J82" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N82" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P82" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y82" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z82" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="4">
+        <v>19</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J83" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N83" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P83" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q83" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z83" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="4">
+        <v>2</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J84" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L84" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N84" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P84" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q84" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y84" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z84" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="4">
+        <v>2</v>
+      </c>
+      <c r="C85" s="4">
+        <v>2</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J85" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L85" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M85" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N85" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P85" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q85" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z85" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC85" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" s="4">
+        <v>2</v>
+      </c>
+      <c r="C86" s="4">
+        <v>3</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P86" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q86" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC86" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B87" s="4">
+        <v>2</v>
+      </c>
+      <c r="C87" s="4">
+        <v>4</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J87" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q87" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="S87" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z87" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B88" s="4">
+        <v>2</v>
+      </c>
+      <c r="C88" s="4">
+        <v>5</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J88" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K88" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M88" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P88" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q88" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="S88" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z88" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B89" s="4">
+        <v>2</v>
+      </c>
+      <c r="C89" s="4">
+        <v>6</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J89" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M89" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N89" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q89" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z89" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90" s="4">
+        <v>2</v>
+      </c>
+      <c r="C90" s="4">
+        <v>7</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K90" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N90" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P90" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q90" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z90" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="4">
+        <v>2</v>
+      </c>
+      <c r="C91" s="4">
+        <v>8</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J91" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K91" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L91" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M91" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N91" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P91" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q91" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z91" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="4">
+        <v>2</v>
+      </c>
+      <c r="C92" s="4">
+        <v>9</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L92" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N92" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P92" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q92" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z92" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" ht="85" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B93" s="4">
+        <v>2</v>
+      </c>
+      <c r="C93" s="4">
+        <v>10</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J93" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M93" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N93" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P93" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q93" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y93" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z93" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" ht="68" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="4">
+        <v>2</v>
+      </c>
+      <c r="C94" s="4">
+        <v>11</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J94" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N94" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P94" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q94" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y94" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z94" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" s="4">
+        <v>2</v>
+      </c>
+      <c r="C95" s="4">
+        <v>12</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J95" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L95" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N95" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P95" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q95" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z95" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="4">
+        <v>2</v>
+      </c>
+      <c r="C96" s="4">
+        <v>13</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J96" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L96" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N96" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P96" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q96" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z96" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B97" s="4">
+        <v>2</v>
+      </c>
+      <c r="C97" s="4">
+        <v>14</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J97" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L97" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M97" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N97" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P97" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q97" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z97" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B98" s="4">
+        <v>2</v>
+      </c>
+      <c r="C98" s="4">
+        <v>15</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J98" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L98" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N98" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P98" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q98" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z98" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B99" s="4">
+        <v>3</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J99" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K99" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L99" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M99" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N99" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P99" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q99" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z99" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B100" s="4">
+        <v>3</v>
+      </c>
+      <c r="C100" s="4">
+        <v>2</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J100" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L100" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M100" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N100" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P100" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q100" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z100" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B101" s="4">
+        <v>3</v>
+      </c>
+      <c r="C101" s="4">
+        <v>3</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J101" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K101" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L101" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M101" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N101" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P101" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q101" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z101" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" s="4">
+        <v>3</v>
+      </c>
+      <c r="C102" s="4">
+        <v>4</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J102" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L102" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N102" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P102" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q102" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z102" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B103" s="4">
+        <v>3</v>
+      </c>
+      <c r="C103" s="4">
+        <v>5</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J103" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K103" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L103" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M103" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N103" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P103" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q103" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z103" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" s="4">
+        <v>3</v>
+      </c>
+      <c r="C104" s="4">
+        <v>6</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J104" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K104" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L104" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N104" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P104" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q104" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z104" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" s="4">
+        <v>3</v>
+      </c>
+      <c r="C105" s="4">
+        <v>7</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J105" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L105" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M105" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N105" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P105" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q105" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z105" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" s="4">
+        <v>3</v>
+      </c>
+      <c r="C106" s="4">
+        <v>8</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J106" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K106" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L106" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N106" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P106" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q106" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z106" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" s="4">
+        <v>3</v>
+      </c>
+      <c r="C107" s="4">
+        <v>9</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J107" s="4">
+        <v>19960925</v>
+      </c>
+      <c r="K107" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L107" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M107" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N107" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="P107" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q107" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z107" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" s="4">
+        <v>3</v>
+      </c>
+      <c r="C108" s="4">
+        <v>10</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J108" s="4">
+        <v>19961030</v>
+      </c>
+      <c r="K108" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="L108" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N108" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P108" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q108" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="S108" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y108" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z108" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" s="4">
+        <v>3</v>
+      </c>
+      <c r="C109" s="4">
+        <v>11</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J109" s="4">
+        <v>19961030</v>
+      </c>
+      <c r="K109" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="L109" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M109" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N109" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O109" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P109" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="X109" s="4">
+        <v>3</v>
+      </c>
+      <c r="Z109" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B110" s="4">
+        <v>3</v>
+      </c>
+      <c r="C110" s="4">
+        <v>12</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I110" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J110" s="4">
+        <v>19961030</v>
+      </c>
+      <c r="K110" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="L110" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N110" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P110" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="X110" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z110" s="4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>